<commit_message>
Entendendo autenticação com JWT java springboot ...
</commit_message>
<xml_diff>
--- a/spring1/registroDeProcedimentos_construcaoDaAplicacao_spring1.xlsx
+++ b/spring1/registroDeProcedimentos_construcaoDaAplicacao_spring1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ERROS DE REQUISIÇÃO HTTP</t>
   </si>
@@ -41,6 +41,14 @@
   </si>
   <si>
     <t>401 - Unauthorized</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;!--Import Google Icon Font--&gt;
+&lt;link href="https://fonts.googleapis.com/icon?family=Material+Icons" rel="stylesheet"&gt;
+&lt;!--Import materialize.css--&gt;
+&lt;link type="text/css" rel="stylesheet" href="materialize/css/materializecss"  media="screen,projection"/&gt;
+&lt;link type="text/css" rel="stylesheet" href="materialize.min.css"  media="screen,projection"/&gt;
+</t>
   </si>
 </sst>
 </file>
@@ -90,12 +98,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,7 +417,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +461,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" s="2"/>
     </row>

</xml_diff>